<commit_message>
actualizacn andre y luis
</commit_message>
<xml_diff>
--- a/OperadoraNominas/bin/Debug/Archivos/timbrado_atl_q.xlsx
+++ b/OperadoraNominas/bin/Debug/Archivos/timbrado_atl_q.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12345" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Generales" sheetId="2" r:id="rId1"/>
@@ -261,7 +261,7 @@
     <author>Omar</author>
   </authors>
   <commentList>
-    <comment ref="I3" authorId="0" shapeId="0">
+    <comment ref="H3" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -282,7 +282,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="169">
   <si>
     <t>No. Empleado</t>
   </si>
@@ -314,6 +314,12 @@
     <t>Ent. Federativa</t>
   </si>
   <si>
+    <t>Días Pagados</t>
+  </si>
+  <si>
+    <t>FechaInicioRelLaboral</t>
+  </si>
+  <si>
     <t>TipoContrato</t>
   </si>
   <si>
@@ -344,69 +350,66 @@
     <t>Subcontratacion</t>
   </si>
   <si>
-    <t>137/001</t>
-  </si>
-  <si>
-    <t>136/001</t>
-  </si>
-  <si>
-    <t>161/002</t>
-  </si>
-  <si>
-    <t>135/019</t>
-  </si>
-  <si>
-    <t>134/019</t>
-  </si>
-  <si>
-    <t>154/020</t>
-  </si>
-  <si>
-    <t>160/021</t>
-  </si>
-  <si>
-    <t>152/038</t>
-  </si>
-  <si>
-    <t>133/038</t>
-  </si>
-  <si>
-    <t>155/038</t>
-  </si>
-  <si>
-    <t>275/038</t>
-  </si>
-  <si>
-    <t>156/038</t>
-  </si>
-  <si>
-    <t>157/038</t>
-  </si>
-  <si>
-    <t>158/038</t>
-  </si>
-  <si>
-    <t>159/038</t>
-  </si>
-  <si>
-    <t>162/038</t>
-  </si>
-  <si>
-    <t>271/038</t>
-  </si>
-  <si>
-    <t>272/038</t>
-  </si>
-  <si>
-    <t>153/038</t>
+    <t>175/001</t>
+  </si>
+  <si>
+    <t>176/001</t>
+  </si>
+  <si>
+    <t>189/002</t>
+  </si>
+  <si>
+    <t>174/019</t>
+  </si>
+  <si>
+    <t>173/019</t>
+  </si>
+  <si>
+    <t>193/020</t>
+  </si>
+  <si>
+    <t>188/021</t>
+  </si>
+  <si>
+    <t>190/038</t>
+  </si>
+  <si>
+    <t>172/038</t>
+  </si>
+  <si>
+    <t>192/038</t>
+  </si>
+  <si>
+    <t>194/038</t>
+  </si>
+  <si>
+    <t>195/038</t>
+  </si>
+  <si>
+    <t>196/038</t>
+  </si>
+  <si>
+    <t>197/038</t>
+  </si>
+  <si>
+    <t>198/038</t>
+  </si>
+  <si>
+    <t>267/038</t>
+  </si>
+  <si>
+    <t>268/038</t>
+  </si>
+  <si>
+    <t>191/038</t>
+  </si>
+  <si>
+    <t>Sueldo</t>
   </si>
   <si>
     <t>Septimo día</t>
   </si>
   <si>
-    <t>Sueldo</t>
-  </si>
-  <si>
     <t>Aguinaldo</t>
   </si>
   <si>
@@ -422,42 +425,39 @@
     <t>Prima vacacional</t>
   </si>
   <si>
+    <t>Vacaciones proporcionales</t>
+  </si>
+  <si>
+    <t>Compensación</t>
+  </si>
+  <si>
+    <t>Dia festivo laborado</t>
+  </si>
+  <si>
+    <t>Bono asistencia</t>
+  </si>
+  <si>
+    <t>Bono productividad</t>
+  </si>
+  <si>
+    <t>Bono polivalencia</t>
+  </si>
+  <si>
+    <t>Bono especialidad</t>
+  </si>
+  <si>
+    <t>Sueldo pendiente</t>
+  </si>
+  <si>
+    <t>APORT PATRONAL PLAN FLEX LP</t>
+  </si>
+  <si>
+    <t>PREVISION_ PFB</t>
+  </si>
+  <si>
     <t>Descanso laborado</t>
   </si>
   <si>
-    <t>Compensación</t>
-  </si>
-  <si>
-    <t>Bono asistencia</t>
-  </si>
-  <si>
-    <t>Bono Calidad</t>
-  </si>
-  <si>
-    <t>Bono productividad</t>
-  </si>
-  <si>
-    <t>Bono polivalencia</t>
-  </si>
-  <si>
-    <t>Bono especialidad</t>
-  </si>
-  <si>
-    <t>Sueldo pendiente</t>
-  </si>
-  <si>
-    <t>Vacaciones proporcionales</t>
-  </si>
-  <si>
-    <t>APORT PATRONAL PLAN FLEX LP</t>
-  </si>
-  <si>
-    <t>PREVISION_ PFB</t>
-  </si>
-  <si>
-    <t>Dia festivo laborado</t>
-  </si>
-  <si>
     <t>Gravado</t>
   </si>
   <si>
@@ -476,69 +476,63 @@
     <t>Importe</t>
   </si>
   <si>
-    <t>138/001</t>
-  </si>
-  <si>
-    <t>146/002</t>
-  </si>
-  <si>
-    <t>274/003</t>
-  </si>
-  <si>
-    <t>273/003</t>
-  </si>
-  <si>
-    <t>165/004</t>
-  </si>
-  <si>
-    <t>167/006</t>
-  </si>
-  <si>
-    <t>147/007</t>
-  </si>
-  <si>
-    <t>148/009</t>
-  </si>
-  <si>
-    <t>142/009</t>
-  </si>
-  <si>
-    <t>141/009</t>
-  </si>
-  <si>
-    <t>140/009</t>
-  </si>
-  <si>
-    <t>139/009</t>
-  </si>
-  <si>
-    <t>143/011</t>
-  </si>
-  <si>
-    <t>144/012</t>
-  </si>
-  <si>
-    <t>166/019</t>
-  </si>
-  <si>
-    <t>163/020</t>
-  </si>
-  <si>
-    <t>164/020</t>
-  </si>
-  <si>
-    <t>Imss</t>
+    <t>185/002</t>
+  </si>
+  <si>
+    <t>269/003</t>
+  </si>
+  <si>
+    <t>270/003</t>
+  </si>
+  <si>
+    <t>204/004</t>
+  </si>
+  <si>
+    <t>206/006</t>
+  </si>
+  <si>
+    <t>186/007</t>
+  </si>
+  <si>
+    <t>180/009</t>
+  </si>
+  <si>
+    <t>181/009</t>
+  </si>
+  <si>
+    <t>179/009</t>
+  </si>
+  <si>
+    <t>178/009</t>
+  </si>
+  <si>
+    <t>187/009</t>
+  </si>
+  <si>
+    <t>182/011</t>
+  </si>
+  <si>
+    <t>183/012</t>
+  </si>
+  <si>
+    <t>205/019</t>
+  </si>
+  <si>
+    <t>203/020</t>
+  </si>
+  <si>
+    <t>202/020</t>
   </si>
   <si>
     <t>I.S.R.</t>
   </si>
   <si>
+    <t>PLAN FLEX LP</t>
+  </si>
+  <si>
     <t>APOR PATRON PLAN FLEX LP</t>
   </si>
   <si>
-    <t>PLAN FLEX LP</t>
-  </si>
-  <si>
     <t>Tiempo no laborado</t>
   </si>
   <si>
@@ -548,21 +542,21 @@
     <t>Pension alimenticia</t>
   </si>
   <si>
+    <t>Prestamo infonavit PORC</t>
+  </si>
+  <si>
+    <t>Seguro de vivienda</t>
+  </si>
+  <si>
+    <t>Prestamo infonavit FD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prestamo Infonavit </t>
+  </si>
+  <si>
     <t>Infonavit Bim Ant</t>
   </si>
   <si>
-    <t>Seguro de vivienda</t>
-  </si>
-  <si>
-    <t>Prestamo infonavit PORC</t>
-  </si>
-  <si>
-    <t>Prestamo infonavit FD</t>
-  </si>
-  <si>
-    <t>Prestamo Infonavit</t>
-  </si>
-  <si>
     <t>Fonacot</t>
   </si>
   <si>
@@ -572,16 +566,16 @@
     <t>Cuota sindical</t>
   </si>
   <si>
+    <t>Permiso sin goce de sueldo</t>
+  </si>
+  <si>
     <t>Faltas injustificadas</t>
   </si>
   <si>
-    <t>Permiso sin goce de sueldo</t>
-  </si>
-  <si>
     <t>Dias Incapacidad</t>
   </si>
   <si>
-    <t>145/002</t>
+    <t>184/002</t>
   </si>
   <si>
     <t>Subsidio</t>
@@ -590,16 +584,172 @@
     <t>Subsidio Causado</t>
   </si>
   <si>
-    <t>Días Pagados</t>
-  </si>
-  <si>
-    <t>FechaInicioRelLaboral</t>
-  </si>
-  <si>
-    <t>276/009</t>
-  </si>
-  <si>
-    <t>Reembolso infonavit</t>
+    <t>DANIEL OLIVARES ARANDA</t>
+  </si>
+  <si>
+    <t>HELC7508164P6</t>
+  </si>
+  <si>
+    <t>CLAUDIA ALEJANDRA HERNANDEZ LOZANO</t>
+  </si>
+  <si>
+    <t>SEGV710823BG7</t>
+  </si>
+  <si>
+    <t>VICTOR MANUEL SEGURA GONZALEZ</t>
+  </si>
+  <si>
+    <t>OIAD7402168ZA</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>19</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>24</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>26</t>
+  </si>
+  <si>
+    <t>27</t>
+  </si>
+  <si>
+    <t>28</t>
+  </si>
+  <si>
+    <t>29</t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
+    <t>31</t>
+  </si>
+  <si>
+    <t>32</t>
+  </si>
+  <si>
+    <t>33</t>
+  </si>
+  <si>
+    <t>34</t>
+  </si>
+  <si>
+    <t>35</t>
+  </si>
+  <si>
+    <t>36</t>
+  </si>
+  <si>
+    <t>37</t>
+  </si>
+  <si>
+    <t>38</t>
+  </si>
+  <si>
+    <t>39</t>
+  </si>
+  <si>
+    <t>40</t>
+  </si>
+  <si>
+    <t>43</t>
+  </si>
+  <si>
+    <t>44</t>
+  </si>
+  <si>
+    <t>45</t>
+  </si>
+  <si>
+    <t>46</t>
+  </si>
+  <si>
+    <t>47</t>
+  </si>
+  <si>
+    <t>48</t>
+  </si>
+  <si>
+    <t>49</t>
+  </si>
+  <si>
+    <t>50</t>
+  </si>
+  <si>
+    <t>277/029</t>
+  </si>
+  <si>
+    <t>Vales de despensa</t>
   </si>
   <si>
     <t>Deducciones</t>
@@ -630,16 +780,26 @@
   </si>
   <si>
     <t>email</t>
+  </si>
+  <si>
+    <t>328/004</t>
+  </si>
+  <si>
+    <t>Vales de despensa D</t>
+  </si>
+  <si>
+    <t>Vales de despensa d</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="\ #,##0.00"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -684,8 +844,14 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -713,11 +879,29 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor rgb="FFDCDCDC"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFF5F5F5"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="19">
+  <borders count="27">
     <border>
       <left/>
       <right/>
@@ -767,32 +951,32 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left style="thick">
         <color rgb="FF000000"/>
       </left>
       <right style="thin">
-        <color rgb="FF000000"/>
+        <color rgb="FF808080"/>
       </right>
       <top style="thin">
-        <color rgb="FF000000"/>
+        <color rgb="FF808080"/>
       </top>
-      <bottom style="thin">
+      <bottom style="thick">
         <color rgb="FF000000"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF000000"/>
+        <color rgb="FF808080"/>
       </left>
-      <right style="thin">
-        <color rgb="FF808080"/>
+      <right style="thick">
+        <color rgb="FF000000"/>
       </right>
       <top style="thin">
         <color rgb="FF808080"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF808080"/>
+      <bottom style="thick">
+        <color rgb="FF000000"/>
       </bottom>
       <diagonal/>
     </border>
@@ -801,18 +985,63 @@
         <color rgb="FF808080"/>
       </left>
       <right style="thin">
-        <color rgb="FF000000"/>
+        <color rgb="FF808080"/>
       </right>
       <top style="thin">
         <color rgb="FF808080"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF808080"/>
+      <bottom style="thick">
+        <color rgb="FF000000"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF808080"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF808080"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF808080"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF808080"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF808080"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF808080"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FF808080"/>
       </left>
       <right style="thin">
@@ -902,14 +1131,14 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left style="thick">
         <color rgb="FF000000"/>
       </left>
-      <right style="thin">
+      <right style="thick">
         <color rgb="FF000000"/>
       </right>
-      <top style="thin">
-        <color rgb="FF808080"/>
+      <top style="thick">
+        <color rgb="FF000000"/>
       </top>
       <bottom style="thin">
         <color rgb="FF808080"/>
@@ -923,8 +1152,8 @@
       <right style="thick">
         <color rgb="FF000000"/>
       </right>
-      <top style="thick">
-        <color rgb="FF000000"/>
+      <top style="thin">
+        <color rgb="FF808080"/>
       </top>
       <bottom style="thin">
         <color rgb="FF808080"/>
@@ -932,10 +1161,75 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thick">
+      <left style="thin">
         <color rgb="FF000000"/>
       </left>
-      <right style="thick">
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF808080"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF808080"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF808080"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF808080"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF808080"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF808080"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF808080"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF808080"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
         <color rgb="FF000000"/>
       </right>
       <top style="thin">
@@ -986,62 +1280,71 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0"/>
     <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyProtection="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="0" fillId="2" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="2" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyProtection="1"/>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1050,16 +1353,40 @@
     <xf numFmtId="49" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1365,14 +1692,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:AF36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="T2" activePane="bottomRight" state="frozenSplit"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="X2" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="U1" sqref="U1:V1"/>
+      <selection pane="bottomRight" activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1383,219 +1709,510 @@
     <col min="4" max="4" width="22.7109375" customWidth="1"/>
     <col min="5" max="5" width="12.7109375" customWidth="1"/>
     <col min="6" max="6" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="9.7109375" customWidth="1"/>
+    <col min="7" max="7" width="9.7109375" customWidth="1"/>
+    <col min="8" max="8" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15.7109375" customWidth="1"/>
     <col min="10" max="11" width="14.7109375" customWidth="1"/>
-    <col min="12" max="12" width="12.7109375" customWidth="1"/>
-    <col min="13" max="13" width="20.7109375" style="18" customWidth="1"/>
-    <col min="14" max="14" width="9.7109375" customWidth="1"/>
+    <col min="12" max="12" width="16.42578125" customWidth="1"/>
+    <col min="13" max="13" width="20.7109375" customWidth="1"/>
+    <col min="14" max="14" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="43" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="13.7109375" customWidth="1"/>
     <col min="17" max="17" width="5.7109375" customWidth="1"/>
     <col min="18" max="18" width="8.7109375" customWidth="1"/>
     <col min="19" max="19" width="6.7109375" customWidth="1"/>
     <col min="20" max="20" width="15.7109375" customWidth="1"/>
-    <col min="21" max="21" width="11.5703125" customWidth="1"/>
-    <col min="22" max="22" width="29.7109375" customWidth="1"/>
-    <col min="23" max="23" width="23" customWidth="1"/>
-    <col min="24" max="24" width="16.5703125" customWidth="1"/>
-    <col min="25" max="25" width="9.7109375" customWidth="1"/>
-    <col min="26" max="26" width="11.7109375" customWidth="1"/>
+    <col min="21" max="21" width="17.7109375" customWidth="1"/>
+    <col min="22" max="22" width="32.85546875" customWidth="1"/>
+    <col min="23" max="23" width="22" customWidth="1"/>
+    <col min="24" max="24" width="16.42578125" customWidth="1"/>
+    <col min="25" max="26" width="9.7109375" customWidth="1"/>
     <col min="27" max="27" width="5.7109375" customWidth="1"/>
     <col min="28" max="28" width="19.7109375" customWidth="1"/>
     <col min="29" max="29" width="16.7109375" customWidth="1"/>
     <col min="30" max="30" width="15.7109375" customWidth="1"/>
-    <col min="31" max="32" width="9.140625" customWidth="1"/>
+    <col min="31" max="31" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:32" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="31" t="s">
+      <c r="B1" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="31" t="s">
+      <c r="C1" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="31" t="s">
+      <c r="D1" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="32" t="s">
+      <c r="E1" s="44" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="33" t="s">
-        <v>114</v>
-      </c>
-      <c r="G1" s="34"/>
-      <c r="H1" s="32" t="s">
+      <c r="F1" s="52" t="s">
+        <v>164</v>
+      </c>
+      <c r="G1" s="53"/>
+      <c r="H1" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="31" t="s">
+      <c r="I1" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="31" t="s">
+      <c r="J1" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="31" t="s">
+      <c r="K1" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="35" t="s">
+      <c r="L1" s="45" t="s">
         <v>9</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="N1" s="31" t="s">
-        <v>102</v>
-      </c>
-      <c r="O1" s="31" t="s">
-        <v>103</v>
-      </c>
-      <c r="P1" s="36" t="s">
+        <v>163</v>
+      </c>
+      <c r="N1" s="43" t="s">
         <v>10</v>
       </c>
-      <c r="Q1" s="37"/>
-      <c r="R1" s="31" t="s">
+      <c r="O1" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="S1" s="36" t="s">
+      <c r="P1" s="54" t="s">
         <v>12</v>
       </c>
-      <c r="T1" s="37"/>
-      <c r="U1" s="36" t="s">
+      <c r="Q1" s="55"/>
+      <c r="R1" s="43" t="s">
         <v>13</v>
       </c>
-      <c r="V1" s="37"/>
-      <c r="W1" s="31" t="s">
+      <c r="S1" s="54" t="s">
         <v>14</v>
       </c>
-      <c r="X1" s="31" t="s">
+      <c r="T1" s="55"/>
+      <c r="U1" s="54" t="s">
         <v>15</v>
       </c>
-      <c r="Y1" s="36" t="s">
+      <c r="V1" s="55"/>
+      <c r="W1" s="43" t="s">
         <v>16</v>
       </c>
-      <c r="Z1" s="37"/>
-      <c r="AA1" s="36" t="s">
+      <c r="X1" s="43" t="s">
         <v>17</v>
       </c>
-      <c r="AB1" s="37"/>
-      <c r="AC1" s="36" t="s">
+      <c r="Y1" s="54" t="s">
         <v>18</v>
       </c>
-      <c r="AD1" s="37"/>
-      <c r="AE1" s="31" t="s">
+      <c r="Z1" s="55"/>
+      <c r="AA1" s="54" t="s">
         <v>19</v>
       </c>
-      <c r="AF1" s="38" t="s">
-        <v>115</v>
+      <c r="AB1" s="55"/>
+      <c r="AC1" s="54" t="s">
+        <v>20</v>
+      </c>
+      <c r="AD1" s="55"/>
+      <c r="AE1" s="43" t="s">
+        <v>21</v>
+      </c>
+      <c r="AF1" s="46" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="2" spans="1:32" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="K2" s="21"/>
+      <c r="A2" s="21"/>
+      <c r="B2" s="22"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="26"/>
+      <c r="K2" s="38"/>
+      <c r="M2" s="23"/>
+      <c r="U2" s="22"/>
+      <c r="V2" s="22"/>
+      <c r="AA2" s="22"/>
     </row>
     <row r="3" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="K3" s="22"/>
+      <c r="A3" s="21"/>
+      <c r="B3" s="22"/>
+      <c r="C3" s="22"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="22"/>
+      <c r="G3" s="27"/>
+      <c r="H3" s="27"/>
+      <c r="K3" s="36"/>
+      <c r="M3" s="23"/>
+      <c r="U3" s="22"/>
+      <c r="V3" s="22"/>
+      <c r="AA3" s="22"/>
     </row>
     <row r="4" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="K4" s="22"/>
+      <c r="A4" s="21"/>
+      <c r="B4" s="22"/>
+      <c r="C4" s="22"/>
+      <c r="D4" s="22"/>
+      <c r="E4" s="22"/>
+      <c r="F4" s="22"/>
+      <c r="G4" s="27"/>
+      <c r="H4" s="27"/>
+      <c r="K4" s="36"/>
+      <c r="M4" s="23"/>
+      <c r="U4" s="22"/>
+      <c r="V4" s="22"/>
+      <c r="AA4" s="22"/>
     </row>
     <row r="5" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="K5" s="22"/>
+      <c r="A5" s="24"/>
+      <c r="B5" s="25"/>
+      <c r="C5" s="25"/>
+      <c r="D5" s="25"/>
+      <c r="E5" s="25"/>
+      <c r="F5" s="22"/>
+      <c r="G5" s="28"/>
+      <c r="H5" s="28"/>
+      <c r="K5" s="36"/>
+      <c r="M5" s="29"/>
+      <c r="U5" s="25"/>
+      <c r="V5" s="25"/>
+      <c r="AA5" s="25"/>
     </row>
     <row r="6" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="K6" s="22"/>
+      <c r="A6" s="24"/>
+      <c r="B6" s="25"/>
+      <c r="C6" s="25"/>
+      <c r="D6" s="25"/>
+      <c r="E6" s="25"/>
+      <c r="F6" s="25"/>
+      <c r="G6" s="28"/>
+      <c r="H6" s="28"/>
+      <c r="K6" s="36"/>
+      <c r="M6" s="29"/>
+      <c r="U6" s="25"/>
+      <c r="V6" s="25"/>
+      <c r="AA6" s="25"/>
     </row>
     <row r="7" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="K7" s="22"/>
+      <c r="A7" s="24"/>
+      <c r="B7" s="25"/>
+      <c r="C7" s="25"/>
+      <c r="D7" s="25"/>
+      <c r="E7" s="25"/>
+      <c r="F7" s="25"/>
+      <c r="G7" s="28"/>
+      <c r="H7" s="28"/>
+      <c r="K7" s="36"/>
+      <c r="M7" s="29"/>
+      <c r="U7" s="25"/>
+      <c r="V7" s="25"/>
+      <c r="AA7" s="25"/>
     </row>
     <row r="8" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="K8" s="22"/>
+      <c r="A8" s="24"/>
+      <c r="B8" s="25"/>
+      <c r="C8" s="25"/>
+      <c r="D8" s="25"/>
+      <c r="E8" s="25"/>
+      <c r="F8" s="25"/>
+      <c r="G8" s="28"/>
+      <c r="H8" s="28"/>
+      <c r="K8" s="36"/>
+      <c r="M8" s="29"/>
+      <c r="U8" s="25"/>
+      <c r="V8" s="25"/>
+      <c r="AA8" s="25"/>
     </row>
     <row r="9" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="K9" s="22"/>
+      <c r="A9" s="24"/>
+      <c r="B9" s="25"/>
+      <c r="C9" s="25"/>
+      <c r="D9" s="25"/>
+      <c r="E9" s="25"/>
+      <c r="F9" s="25"/>
+      <c r="G9" s="28"/>
+      <c r="H9" s="28"/>
+      <c r="K9" s="36"/>
+      <c r="M9" s="29"/>
+      <c r="U9" s="25"/>
+      <c r="V9" s="25"/>
+      <c r="AA9" s="25"/>
     </row>
     <row r="10" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="K10" s="22"/>
+      <c r="A10" s="24"/>
+      <c r="B10" s="25"/>
+      <c r="C10" s="25"/>
+      <c r="D10" s="25"/>
+      <c r="E10" s="25"/>
+      <c r="F10" s="25"/>
+      <c r="G10" s="28"/>
+      <c r="H10" s="28"/>
+      <c r="K10" s="36"/>
+      <c r="M10" s="29"/>
+      <c r="U10" s="25"/>
+      <c r="V10" s="25"/>
+      <c r="AA10" s="25"/>
     </row>
     <row r="11" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="K11" s="22"/>
+      <c r="A11" s="24"/>
+      <c r="B11" s="25"/>
+      <c r="C11" s="25"/>
+      <c r="D11" s="25"/>
+      <c r="E11" s="25"/>
+      <c r="F11" s="25"/>
+      <c r="G11" s="28"/>
+      <c r="H11" s="28"/>
+      <c r="K11" s="36"/>
+      <c r="M11" s="29"/>
+      <c r="U11" s="25"/>
+      <c r="V11" s="25"/>
+      <c r="AA11" s="25"/>
     </row>
     <row r="12" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="K12" s="22"/>
+      <c r="A12" s="24"/>
+      <c r="B12" s="25"/>
+      <c r="C12" s="25"/>
+      <c r="D12" s="25"/>
+      <c r="E12" s="25"/>
+      <c r="F12" s="25"/>
+      <c r="G12" s="28"/>
+      <c r="H12" s="28"/>
+      <c r="K12" s="36"/>
+      <c r="M12" s="29"/>
+      <c r="U12" s="25"/>
+      <c r="V12" s="25"/>
+      <c r="AA12" s="25"/>
     </row>
     <row r="13" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="K13" s="22"/>
+      <c r="A13" s="24"/>
+      <c r="B13" s="25"/>
+      <c r="C13" s="25"/>
+      <c r="D13" s="25"/>
+      <c r="E13" s="25"/>
+      <c r="F13" s="25"/>
+      <c r="G13" s="28"/>
+      <c r="H13" s="28"/>
+      <c r="K13" s="36"/>
+      <c r="M13" s="29"/>
+      <c r="U13" s="25"/>
+      <c r="V13" s="25"/>
+      <c r="AA13" s="25"/>
     </row>
     <row r="14" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="K14" s="22"/>
+      <c r="A14" s="24"/>
+      <c r="B14" s="25"/>
+      <c r="C14" s="25"/>
+      <c r="D14" s="25"/>
+      <c r="E14" s="25"/>
+      <c r="F14" s="25"/>
+      <c r="G14" s="28"/>
+      <c r="H14" s="28"/>
+      <c r="K14" s="36"/>
+      <c r="M14" s="29"/>
+      <c r="U14" s="25"/>
+      <c r="V14" s="25"/>
+      <c r="AA14" s="25"/>
     </row>
     <row r="15" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="K15" s="22"/>
+      <c r="A15" s="24"/>
+      <c r="B15" s="25"/>
+      <c r="C15" s="25"/>
+      <c r="D15" s="25"/>
+      <c r="E15" s="25"/>
+      <c r="F15" s="25"/>
+      <c r="G15" s="28"/>
+      <c r="H15" s="28"/>
+      <c r="K15" s="36"/>
+      <c r="M15" s="29"/>
+      <c r="U15" s="25"/>
+      <c r="V15" s="25"/>
+      <c r="AA15" s="25"/>
     </row>
     <row r="16" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="K16" s="22"/>
-    </row>
-    <row r="17" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K17" s="22"/>
-    </row>
-    <row r="18" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K18" s="22"/>
-    </row>
-    <row r="19" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K19" s="22"/>
-    </row>
-    <row r="20" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K20" s="22"/>
-    </row>
-    <row r="21" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K21" s="22"/>
-    </row>
-    <row r="22" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K22" s="22"/>
-    </row>
-    <row r="23" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K23" s="22"/>
-    </row>
-    <row r="24" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K24" s="22"/>
-    </row>
-    <row r="25" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K25" s="22"/>
-    </row>
-    <row r="26" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K26" s="22"/>
-    </row>
-    <row r="27" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K27" s="22"/>
-    </row>
-    <row r="28" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K28" s="22"/>
-    </row>
-    <row r="29" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K29" s="22"/>
-    </row>
-    <row r="30" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K30" s="22"/>
-    </row>
-    <row r="31" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K31" s="22"/>
-    </row>
-    <row r="32" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K32" s="22"/>
+      <c r="A16" s="24"/>
+      <c r="B16" s="25"/>
+      <c r="C16" s="25"/>
+      <c r="D16" s="25"/>
+      <c r="E16" s="25"/>
+      <c r="F16" s="25"/>
+      <c r="G16" s="28"/>
+      <c r="H16" s="28"/>
+      <c r="K16" s="36"/>
+      <c r="M16" s="29"/>
+      <c r="U16" s="25"/>
+      <c r="V16" s="25"/>
+      <c r="AA16" s="25"/>
+    </row>
+    <row r="17" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A17" s="24"/>
+      <c r="B17" s="25"/>
+      <c r="C17" s="25"/>
+      <c r="D17" s="25"/>
+      <c r="E17" s="25"/>
+      <c r="F17" s="25"/>
+      <c r="G17" s="28"/>
+      <c r="H17" s="28"/>
+      <c r="K17" s="36"/>
+      <c r="M17" s="29"/>
+      <c r="U17" s="25"/>
+      <c r="V17" s="25"/>
+      <c r="AA17" s="25"/>
+    </row>
+    <row r="18" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A18" s="24"/>
+      <c r="B18" s="25"/>
+      <c r="C18" s="25"/>
+      <c r="D18" s="25"/>
+      <c r="E18" s="25"/>
+      <c r="F18" s="25"/>
+      <c r="G18" s="28"/>
+      <c r="H18" s="28"/>
+      <c r="K18" s="36"/>
+      <c r="M18" s="29"/>
+      <c r="U18" s="25"/>
+      <c r="V18" s="25"/>
+      <c r="AA18" s="25"/>
+    </row>
+    <row r="19" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A19" s="24"/>
+      <c r="B19" s="25"/>
+      <c r="C19" s="25"/>
+      <c r="D19" s="25"/>
+      <c r="E19" s="25"/>
+      <c r="F19" s="25"/>
+      <c r="G19" s="28"/>
+      <c r="H19" s="28"/>
+      <c r="K19" s="36"/>
+      <c r="M19" s="29"/>
+      <c r="U19" s="25"/>
+      <c r="V19" s="25"/>
+      <c r="AA19" s="25"/>
+    </row>
+    <row r="20" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A20" s="24"/>
+      <c r="B20" s="25"/>
+      <c r="C20" s="25"/>
+      <c r="D20" s="25"/>
+      <c r="E20" s="25"/>
+      <c r="F20" s="25"/>
+      <c r="G20" s="28"/>
+      <c r="H20" s="28"/>
+      <c r="K20" s="36"/>
+      <c r="M20" s="29"/>
+      <c r="U20" s="25"/>
+      <c r="V20" s="25"/>
+      <c r="AA20" s="25"/>
+    </row>
+    <row r="21" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A21" s="24"/>
+      <c r="B21" s="25"/>
+      <c r="C21" s="25"/>
+      <c r="D21" s="25"/>
+      <c r="E21" s="25"/>
+      <c r="F21" s="25"/>
+      <c r="G21" s="28"/>
+      <c r="H21" s="28"/>
+      <c r="K21" s="36"/>
+      <c r="M21" s="29"/>
+      <c r="U21" s="25"/>
+      <c r="V21" s="25"/>
+      <c r="AA21" s="25"/>
+    </row>
+    <row r="22" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A22" s="24"/>
+      <c r="B22" s="25"/>
+      <c r="C22" s="25"/>
+      <c r="D22" s="25"/>
+      <c r="E22" s="25"/>
+      <c r="F22" s="25"/>
+      <c r="G22" s="28"/>
+      <c r="H22" s="28"/>
+      <c r="K22" s="36"/>
+      <c r="M22" s="29"/>
+      <c r="U22" s="25"/>
+      <c r="V22" s="25"/>
+      <c r="AA22" s="25"/>
+    </row>
+    <row r="23" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A23" s="24"/>
+      <c r="B23" s="25"/>
+      <c r="C23" s="25"/>
+      <c r="D23" s="25"/>
+      <c r="E23" s="25"/>
+      <c r="F23" s="25"/>
+      <c r="G23" s="28"/>
+      <c r="H23" s="28"/>
+      <c r="K23" s="36"/>
+      <c r="M23" s="29"/>
+      <c r="U23" s="25"/>
+      <c r="V23" s="25"/>
+      <c r="AA23" s="25"/>
+    </row>
+    <row r="24" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A24" s="24"/>
+      <c r="B24" s="25"/>
+      <c r="C24" s="25"/>
+      <c r="D24" s="25"/>
+      <c r="E24" s="25"/>
+      <c r="F24" s="25"/>
+      <c r="G24" s="28"/>
+      <c r="H24" s="28"/>
+      <c r="K24" s="36"/>
+      <c r="M24" s="29"/>
+      <c r="U24" s="25"/>
+      <c r="V24" s="25"/>
+      <c r="AA24" s="25"/>
+    </row>
+    <row r="25" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A25" s="24"/>
+      <c r="B25" s="25"/>
+      <c r="C25" s="25"/>
+      <c r="D25" s="25"/>
+      <c r="E25" s="25"/>
+      <c r="F25" s="25"/>
+      <c r="G25" s="28"/>
+      <c r="H25" s="28"/>
+      <c r="K25" s="36"/>
+      <c r="M25" s="29"/>
+      <c r="U25" s="25"/>
+      <c r="V25" s="25"/>
+      <c r="AA25" s="25"/>
+    </row>
+    <row r="26" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="K26" s="36"/>
+      <c r="U26" s="21"/>
+      <c r="V26" s="21"/>
+    </row>
+    <row r="27" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="K27" s="36"/>
+    </row>
+    <row r="28" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="K28" s="36"/>
+    </row>
+    <row r="29" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="K29" s="36"/>
+    </row>
+    <row r="30" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="K30" s="36"/>
+    </row>
+    <row r="31" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="K31" s="36"/>
+    </row>
+    <row r="32" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="K32" s="36"/>
     </row>
     <row r="33" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K33" s="22"/>
+      <c r="K33" s="36"/>
     </row>
     <row r="34" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K34" s="22"/>
+      <c r="K34" s="36"/>
     </row>
     <row r="35" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K35" s="22"/>
+      <c r="K35" s="36"/>
     </row>
     <row r="36" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K36" s="22"/>
+      <c r="K36" s="36"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -1619,14 +2236,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Hoja2"/>
-  <dimension ref="A1:AW3"/>
+  <dimension ref="A1:AW28"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozenSplit"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="2" ySplit="3" topLeftCell="AE7" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A4" sqref="A4:XFD23"/>
+      <selection pane="bottomRight" activeCell="A7" sqref="A7:XFD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1634,350 +2250,800 @@
     <col min="1" max="1" width="17.7109375" customWidth="1"/>
     <col min="2" max="2" width="42.7109375" customWidth="1"/>
     <col min="3" max="20" width="9.140625" customWidth="1"/>
-    <col min="44" max="44" width="20.85546875" customWidth="1"/>
-    <col min="46" max="46" width="10.28515625" customWidth="1"/>
-    <col min="49" max="49" width="9.140625" style="16"/>
+    <col min="25" max="26" width="13.5703125" customWidth="1"/>
+    <col min="42" max="42" width="12" customWidth="1"/>
+    <col min="44" max="44" width="32.42578125" customWidth="1"/>
+    <col min="46" max="46" width="15.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:48" x14ac:dyDescent="0.25">
-      <c r="C1" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D1" s="8"/>
-      <c r="E1" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="F1" s="10"/>
-      <c r="G1" s="7" t="s">
+    <row r="1" spans="1:49" x14ac:dyDescent="0.25">
+      <c r="C1" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="H1" s="8"/>
-      <c r="I1" s="9" t="s">
+      <c r="D1" s="14"/>
+      <c r="E1" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="J1" s="11"/>
-      <c r="K1" s="11"/>
-      <c r="L1" s="11"/>
-      <c r="M1" s="11"/>
-      <c r="N1" s="10"/>
-      <c r="O1" s="7" t="s">
+      <c r="F1" s="16"/>
+      <c r="G1" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="P1" s="12"/>
-      <c r="Q1" s="12"/>
-      <c r="R1" s="12"/>
-      <c r="S1" s="12"/>
-      <c r="T1" s="8"/>
-      <c r="U1" s="9" t="s">
+      <c r="H1" s="14"/>
+      <c r="I1" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="V1" s="10"/>
-      <c r="W1" s="7" t="s">
+      <c r="J1" s="17"/>
+      <c r="K1" s="17"/>
+      <c r="L1" s="17"/>
+      <c r="M1" s="17"/>
+      <c r="N1" s="14"/>
+      <c r="O1" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="X1" s="8"/>
-      <c r="Y1" s="9" t="s">
+      <c r="P1" s="18"/>
+      <c r="Q1" s="18"/>
+      <c r="R1" s="18"/>
+      <c r="S1" s="18"/>
+      <c r="T1" s="16"/>
+      <c r="U1" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="Z1" s="10"/>
-      <c r="AA1" s="7" t="s">
+      <c r="V1" s="14"/>
+      <c r="W1" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="AB1" s="8"/>
-      <c r="AC1" s="9" t="s">
+      <c r="X1" s="16"/>
+      <c r="Y1" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="AD1" s="10"/>
-      <c r="AE1" s="7" t="s">
+      <c r="Z1" s="16"/>
+      <c r="AA1" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="8"/>
-      <c r="AG1" s="9" t="s">
+      <c r="AB1" s="14"/>
+      <c r="AC1" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="AH1" s="10"/>
-      <c r="AI1" s="7" t="s">
+      <c r="AD1" s="16"/>
+      <c r="AE1" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="AJ1" s="8"/>
-      <c r="AK1" s="9" t="s">
+      <c r="AF1" s="14"/>
+      <c r="AG1" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="AL1" s="10"/>
-      <c r="AM1" s="7" t="s">
+      <c r="AH1" s="16"/>
+      <c r="AI1" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="AN1" s="8"/>
-      <c r="AO1" s="9" t="s">
+      <c r="AJ1" s="14"/>
+      <c r="AK1" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="AP1" s="10"/>
-      <c r="AQ1" s="7" t="s">
+      <c r="AL1" s="16"/>
+      <c r="AM1" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="AR1" s="8"/>
-      <c r="AS1" s="9" t="s">
+      <c r="AN1" s="14"/>
+      <c r="AO1" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="AP1" s="16"/>
+      <c r="AQ1" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="AT1" s="10"/>
-      <c r="AU1" s="7" t="s">
+      <c r="AR1" s="16"/>
+      <c r="AS1" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="AV1" s="8"/>
-    </row>
-    <row r="2" spans="1:48" x14ac:dyDescent="0.25">
-      <c r="C2" s="23" t="s">
+      <c r="AT1" s="14"/>
+      <c r="AU1" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="D2" s="24"/>
-      <c r="E2" s="25" t="s">
+      <c r="AV1" s="16"/>
+    </row>
+    <row r="2" spans="1:49" x14ac:dyDescent="0.25">
+      <c r="C2" s="59" t="s">
         <v>40</v>
       </c>
-      <c r="F2" s="26"/>
-      <c r="G2" s="23" t="s">
+      <c r="D2" s="60"/>
+      <c r="E2" s="56" t="s">
         <v>41</v>
       </c>
-      <c r="H2" s="24"/>
-      <c r="I2" s="25" t="s">
+      <c r="F2" s="58"/>
+      <c r="G2" s="59" t="s">
         <v>42</v>
       </c>
-      <c r="J2" s="27"/>
-      <c r="K2" s="27"/>
-      <c r="L2" s="27"/>
-      <c r="M2" s="27"/>
-      <c r="N2" s="26"/>
-      <c r="O2" s="23" t="s">
+      <c r="H2" s="60"/>
+      <c r="I2" s="59" t="s">
         <v>43</v>
       </c>
-      <c r="P2" s="28"/>
-      <c r="Q2" s="28"/>
-      <c r="R2" s="28"/>
-      <c r="S2" s="28"/>
-      <c r="T2" s="24"/>
-      <c r="U2" s="25" t="s">
+      <c r="J2" s="61"/>
+      <c r="K2" s="61"/>
+      <c r="L2" s="61"/>
+      <c r="M2" s="61"/>
+      <c r="N2" s="60"/>
+      <c r="O2" s="56" t="s">
         <v>44</v>
       </c>
-      <c r="V2" s="26"/>
-      <c r="W2" s="23" t="s">
+      <c r="P2" s="57"/>
+      <c r="Q2" s="57"/>
+      <c r="R2" s="57"/>
+      <c r="S2" s="57"/>
+      <c r="T2" s="58"/>
+      <c r="U2" s="59" t="s">
         <v>45</v>
       </c>
-      <c r="X2" s="24"/>
-      <c r="Y2" s="25" t="s">
+      <c r="V2" s="60"/>
+      <c r="W2" s="56" t="s">
         <v>46</v>
       </c>
-      <c r="Z2" s="26"/>
-      <c r="AA2" s="23" t="s">
+      <c r="X2" s="58"/>
+      <c r="Y2" s="56" t="s">
         <v>47</v>
       </c>
-      <c r="AB2" s="24"/>
-      <c r="AC2" s="25" t="s">
+      <c r="Z2" s="58"/>
+      <c r="AA2" s="59" t="s">
         <v>48</v>
       </c>
-      <c r="AD2" s="26"/>
-      <c r="AE2" s="23" t="s">
+      <c r="AB2" s="60"/>
+      <c r="AC2" s="56" t="s">
         <v>49</v>
       </c>
-      <c r="AF2" s="24"/>
-      <c r="AG2" s="25" t="s">
+      <c r="AD2" s="58"/>
+      <c r="AE2" s="59" t="s">
         <v>50</v>
       </c>
-      <c r="AH2" s="26"/>
-      <c r="AI2" s="23" t="s">
+      <c r="AF2" s="60"/>
+      <c r="AG2" s="56" t="s">
         <v>51</v>
       </c>
-      <c r="AJ2" s="24"/>
-      <c r="AK2" s="25" t="s">
+      <c r="AH2" s="58"/>
+      <c r="AI2" s="59" t="s">
         <v>52</v>
       </c>
-      <c r="AL2" s="26"/>
-      <c r="AM2" s="23" t="s">
+      <c r="AJ2" s="60"/>
+      <c r="AK2" s="56" t="s">
         <v>53</v>
       </c>
-      <c r="AN2" s="24"/>
-      <c r="AO2" s="25" t="s">
+      <c r="AL2" s="58"/>
+      <c r="AM2" s="59" t="s">
         <v>54</v>
       </c>
-      <c r="AP2" s="26"/>
-      <c r="AQ2" s="23" t="s">
+      <c r="AN2" s="60"/>
+      <c r="AO2" s="62" t="s">
+        <v>155</v>
+      </c>
+      <c r="AP2" s="63"/>
+      <c r="AQ2" s="56" t="s">
         <v>55</v>
       </c>
-      <c r="AR2" s="24"/>
-      <c r="AS2" s="25" t="s">
+      <c r="AR2" s="58"/>
+      <c r="AS2" s="59" t="s">
         <v>56</v>
       </c>
-      <c r="AT2" s="26"/>
-      <c r="AU2" s="23" t="s">
+      <c r="AT2" s="60"/>
+      <c r="AU2" s="56" t="s">
         <v>57</v>
       </c>
-      <c r="AV2" s="24"/>
-    </row>
-    <row r="3" spans="1:48" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="AV2" s="58"/>
+    </row>
+    <row r="3" spans="1:49" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="G3" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="H3" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="I3" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="J3" s="5" t="s">
+      <c r="J3" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="K3" s="5" t="s">
+      <c r="K3" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="L3" s="6" t="s">
+      <c r="L3" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="M3" s="5" t="s">
+      <c r="M3" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="N3" s="4" t="s">
+      <c r="N3" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="O3" s="3" t="s">
+      <c r="O3" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="P3" s="5" t="s">
+      <c r="P3" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="Q3" s="5" t="s">
+      <c r="Q3" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="R3" s="6" t="s">
+      <c r="R3" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="S3" s="5" t="s">
+      <c r="S3" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="T3" s="4" t="s">
+      <c r="T3" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="U3" s="3" t="s">
+      <c r="U3" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="V3" s="4" t="s">
+      <c r="V3" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="W3" s="3" t="s">
+      <c r="W3" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="X3" s="4" t="s">
+      <c r="X3" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="Y3" s="3" t="s">
+      <c r="Y3" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="Z3" s="4" t="s">
+      <c r="Z3" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="AA3" s="3" t="s">
+      <c r="AA3" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="AB3" s="4" t="s">
+      <c r="AB3" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="AC3" s="3" t="s">
+      <c r="AC3" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="AD3" s="4" t="s">
+      <c r="AD3" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="AE3" s="3" t="s">
+      <c r="AE3" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="AF3" s="4" t="s">
+      <c r="AF3" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="AG3" s="3" t="s">
+      <c r="AG3" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="AH3" s="4" t="s">
+      <c r="AH3" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="AI3" s="3" t="s">
+      <c r="AI3" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="AJ3" s="4" t="s">
+      <c r="AJ3" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="AK3" s="3" t="s">
+      <c r="AK3" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="AL3" s="4" t="s">
+      <c r="AL3" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="AM3" s="3" t="s">
+      <c r="AM3" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="AN3" s="4" t="s">
+      <c r="AN3" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="AO3" s="3" t="s">
+      <c r="AO3" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="AP3" s="4" t="s">
+      <c r="AP3" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="AQ3" s="3" t="s">
+      <c r="AQ3" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="AR3" s="4" t="s">
+      <c r="AR3" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="AS3" s="3" t="s">
+      <c r="AS3" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="AT3" s="4" t="s">
+      <c r="AT3" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="AU3" s="3" t="s">
+      <c r="AU3" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="AV3" s="4" t="s">
+      <c r="AV3" s="10" t="s">
         <v>59</v>
       </c>
+    </row>
+    <row r="4" spans="1:49" x14ac:dyDescent="0.25">
+      <c r="A4" s="22" t="s">
+        <v>105</v>
+      </c>
+      <c r="B4" s="22" t="s">
+        <v>100</v>
+      </c>
+      <c r="C4" s="2">
+        <v>12121.2</v>
+      </c>
+      <c r="D4" s="3"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="6"/>
+      <c r="K4" s="6"/>
+      <c r="L4" s="6"/>
+      <c r="M4" s="6"/>
+      <c r="N4" s="3"/>
+      <c r="O4" s="4"/>
+      <c r="P4" s="7"/>
+      <c r="Q4" s="7"/>
+      <c r="R4" s="7"/>
+      <c r="S4" s="7"/>
+      <c r="T4" s="5"/>
+      <c r="U4" s="27">
+        <v>0</v>
+      </c>
+      <c r="V4" s="27">
+        <v>0</v>
+      </c>
+      <c r="W4" s="21"/>
+      <c r="X4" s="21"/>
+      <c r="Y4" s="4"/>
+      <c r="Z4" s="5"/>
+      <c r="AA4" s="2"/>
+      <c r="AB4" s="3"/>
+      <c r="AD4" s="5"/>
+      <c r="AE4" s="2"/>
+      <c r="AF4" s="3"/>
+      <c r="AG4" s="4"/>
+      <c r="AH4" s="5"/>
+      <c r="AI4" s="2"/>
+      <c r="AJ4" s="3"/>
+      <c r="AK4" s="4"/>
+      <c r="AL4" s="5"/>
+      <c r="AM4" s="2"/>
+      <c r="AN4" s="3"/>
+      <c r="AO4" s="2"/>
+      <c r="AP4" s="3"/>
+      <c r="AQ4" s="4"/>
+      <c r="AR4" s="5"/>
+      <c r="AS4" s="2"/>
+      <c r="AT4" s="3"/>
+      <c r="AU4" s="27">
+        <v>0</v>
+      </c>
+      <c r="AV4" s="5"/>
+      <c r="AW4">
+        <f>SUM(C4:AV4)</f>
+        <v>12121.2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:49" x14ac:dyDescent="0.25">
+      <c r="A5" s="22" t="s">
+        <v>101</v>
+      </c>
+      <c r="B5" s="22" t="s">
+        <v>102</v>
+      </c>
+      <c r="C5">
+        <v>7094.4</v>
+      </c>
+      <c r="U5" s="27">
+        <v>0</v>
+      </c>
+      <c r="V5" s="27">
+        <v>0</v>
+      </c>
+      <c r="W5" s="21"/>
+      <c r="X5" s="21"/>
+      <c r="AU5" s="27">
+        <v>0</v>
+      </c>
+      <c r="AW5">
+        <f t="shared" ref="AW5:AW6" si="0">SUM(C5:AV5)</f>
+        <v>7094.4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:49" x14ac:dyDescent="0.25">
+      <c r="A6" s="22" t="s">
+        <v>103</v>
+      </c>
+      <c r="B6" s="22" t="s">
+        <v>104</v>
+      </c>
+      <c r="C6">
+        <v>7245</v>
+      </c>
+      <c r="U6" s="27">
+        <v>0</v>
+      </c>
+      <c r="V6" s="27">
+        <v>0</v>
+      </c>
+      <c r="W6" s="21"/>
+      <c r="X6" s="21"/>
+      <c r="AU6" s="27">
+        <v>0</v>
+      </c>
+      <c r="AW6">
+        <f t="shared" si="0"/>
+        <v>7245</v>
+      </c>
+    </row>
+    <row r="7" spans="1:49" x14ac:dyDescent="0.25">
+      <c r="A7" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="B7" s="25" t="s">
+        <v>107</v>
+      </c>
+      <c r="C7" s="25" t="s">
+        <v>108</v>
+      </c>
+      <c r="D7" s="25" t="s">
+        <v>109</v>
+      </c>
+      <c r="E7" s="25" t="s">
+        <v>110</v>
+      </c>
+      <c r="F7" s="25" t="s">
+        <v>111</v>
+      </c>
+      <c r="G7" s="25" t="s">
+        <v>112</v>
+      </c>
+      <c r="H7" s="25" t="s">
+        <v>113</v>
+      </c>
+      <c r="I7" s="25" t="s">
+        <v>114</v>
+      </c>
+      <c r="J7" s="25" t="s">
+        <v>115</v>
+      </c>
+      <c r="K7" s="25" t="s">
+        <v>116</v>
+      </c>
+      <c r="L7" s="25" t="s">
+        <v>117</v>
+      </c>
+      <c r="M7" s="25" t="s">
+        <v>118</v>
+      </c>
+      <c r="N7" s="25" t="s">
+        <v>119</v>
+      </c>
+      <c r="O7" s="25" t="s">
+        <v>120</v>
+      </c>
+      <c r="P7" s="25" t="s">
+        <v>121</v>
+      </c>
+      <c r="Q7" s="25" t="s">
+        <v>122</v>
+      </c>
+      <c r="R7" s="25" t="s">
+        <v>123</v>
+      </c>
+      <c r="S7" s="25" t="s">
+        <v>124</v>
+      </c>
+      <c r="T7" s="25" t="s">
+        <v>125</v>
+      </c>
+      <c r="U7" s="25" t="s">
+        <v>126</v>
+      </c>
+      <c r="V7" s="25" t="s">
+        <v>127</v>
+      </c>
+      <c r="W7" s="25" t="s">
+        <v>128</v>
+      </c>
+      <c r="X7" s="25" t="s">
+        <v>129</v>
+      </c>
+      <c r="Y7" s="25" t="s">
+        <v>130</v>
+      </c>
+      <c r="Z7" s="25" t="s">
+        <v>131</v>
+      </c>
+      <c r="AA7" s="25" t="s">
+        <v>132</v>
+      </c>
+      <c r="AB7" s="25" t="s">
+        <v>133</v>
+      </c>
+      <c r="AC7" s="25" t="s">
+        <v>134</v>
+      </c>
+      <c r="AD7" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="AE7" s="25" t="s">
+        <v>136</v>
+      </c>
+      <c r="AF7" s="25" t="s">
+        <v>137</v>
+      </c>
+      <c r="AG7" s="25" t="s">
+        <v>138</v>
+      </c>
+      <c r="AH7" s="25" t="s">
+        <v>139</v>
+      </c>
+      <c r="AI7" s="25" t="s">
+        <v>140</v>
+      </c>
+      <c r="AJ7" s="25" t="s">
+        <v>141</v>
+      </c>
+      <c r="AK7" s="25" t="s">
+        <v>142</v>
+      </c>
+      <c r="AL7" s="25" t="s">
+        <v>143</v>
+      </c>
+      <c r="AM7" s="25" t="s">
+        <v>144</v>
+      </c>
+      <c r="AN7" s="25" t="s">
+        <v>145</v>
+      </c>
+      <c r="AO7" s="25" t="s">
+        <v>146</v>
+      </c>
+      <c r="AP7" s="25" t="s">
+        <v>147</v>
+      </c>
+      <c r="AQ7" s="25" t="s">
+        <v>148</v>
+      </c>
+      <c r="AR7" s="25" t="s">
+        <v>149</v>
+      </c>
+      <c r="AS7" s="25" t="s">
+        <v>150</v>
+      </c>
+      <c r="AT7" s="25" t="s">
+        <v>151</v>
+      </c>
+      <c r="AU7" s="25" t="s">
+        <v>152</v>
+      </c>
+      <c r="AV7" s="25" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="8" spans="1:49" x14ac:dyDescent="0.25">
+      <c r="A8" s="25"/>
+      <c r="B8" s="25"/>
+      <c r="U8" s="28"/>
+      <c r="V8" s="28"/>
+      <c r="W8" s="21"/>
+      <c r="X8" s="21"/>
+      <c r="AU8" s="28"/>
+    </row>
+    <row r="9" spans="1:49" x14ac:dyDescent="0.25">
+      <c r="A9" s="25"/>
+      <c r="B9" s="25"/>
+      <c r="U9" s="28"/>
+      <c r="V9" s="28"/>
+      <c r="W9" s="21"/>
+      <c r="X9" s="21"/>
+      <c r="AU9" s="28"/>
+    </row>
+    <row r="10" spans="1:49" x14ac:dyDescent="0.25">
+      <c r="A10" s="25"/>
+      <c r="B10" s="25"/>
+      <c r="U10" s="28"/>
+      <c r="V10" s="28"/>
+      <c r="W10" s="21"/>
+      <c r="X10" s="21"/>
+      <c r="AU10" s="28"/>
+    </row>
+    <row r="11" spans="1:49" x14ac:dyDescent="0.25">
+      <c r="A11" s="25"/>
+      <c r="B11" s="25"/>
+      <c r="U11" s="28"/>
+      <c r="V11" s="28"/>
+      <c r="W11" s="21"/>
+      <c r="X11" s="21"/>
+      <c r="AU11" s="28"/>
+    </row>
+    <row r="12" spans="1:49" x14ac:dyDescent="0.25">
+      <c r="A12" s="25"/>
+      <c r="B12" s="25"/>
+      <c r="U12" s="28"/>
+      <c r="V12" s="28"/>
+      <c r="W12" s="21"/>
+      <c r="X12" s="21"/>
+      <c r="AU12" s="28"/>
+    </row>
+    <row r="13" spans="1:49" x14ac:dyDescent="0.25">
+      <c r="A13" s="25"/>
+      <c r="B13" s="25"/>
+      <c r="U13" s="28"/>
+      <c r="V13" s="28"/>
+      <c r="W13" s="21"/>
+      <c r="X13" s="21"/>
+      <c r="AU13" s="28"/>
+    </row>
+    <row r="14" spans="1:49" x14ac:dyDescent="0.25">
+      <c r="A14" s="25"/>
+      <c r="B14" s="25"/>
+      <c r="U14" s="28"/>
+      <c r="V14" s="28"/>
+      <c r="W14" s="21"/>
+      <c r="X14" s="21"/>
+      <c r="AU14" s="28"/>
+    </row>
+    <row r="15" spans="1:49" x14ac:dyDescent="0.25">
+      <c r="A15" s="25"/>
+      <c r="B15" s="25"/>
+      <c r="U15" s="28"/>
+      <c r="V15" s="28"/>
+      <c r="W15" s="21"/>
+      <c r="X15" s="21"/>
+      <c r="AU15" s="28"/>
+    </row>
+    <row r="16" spans="1:49" x14ac:dyDescent="0.25">
+      <c r="A16" s="25"/>
+      <c r="B16" s="25"/>
+      <c r="U16" s="28"/>
+      <c r="V16" s="28"/>
+      <c r="W16" s="21"/>
+      <c r="X16" s="21"/>
+      <c r="AU16" s="28"/>
+    </row>
+    <row r="17" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="A17" s="25"/>
+      <c r="B17" s="25"/>
+      <c r="U17" s="28"/>
+      <c r="V17" s="28"/>
+      <c r="W17" s="21"/>
+      <c r="X17" s="21"/>
+      <c r="AU17" s="28"/>
+    </row>
+    <row r="18" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="A18" s="25"/>
+      <c r="B18" s="25"/>
+      <c r="U18" s="28"/>
+      <c r="V18" s="28"/>
+      <c r="W18" s="21"/>
+      <c r="X18" s="21"/>
+      <c r="AU18" s="28"/>
+    </row>
+    <row r="19" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="A19" s="25"/>
+      <c r="B19" s="25"/>
+      <c r="U19" s="28"/>
+      <c r="V19" s="28"/>
+      <c r="W19" s="21"/>
+      <c r="X19" s="21"/>
+      <c r="AU19" s="28"/>
+    </row>
+    <row r="20" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="A20" s="25"/>
+      <c r="B20" s="25"/>
+      <c r="U20" s="28"/>
+      <c r="V20" s="28"/>
+      <c r="W20" s="21"/>
+      <c r="X20" s="21"/>
+      <c r="AU20" s="28"/>
+    </row>
+    <row r="21" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="A21" s="25"/>
+      <c r="B21" s="25"/>
+      <c r="U21" s="28"/>
+      <c r="V21" s="28"/>
+      <c r="W21" s="21"/>
+      <c r="X21" s="21"/>
+      <c r="AU21" s="28"/>
+    </row>
+    <row r="22" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="A22" s="25"/>
+      <c r="B22" s="25"/>
+      <c r="U22" s="28"/>
+      <c r="V22" s="28"/>
+      <c r="W22" s="21"/>
+      <c r="X22" s="21"/>
+      <c r="AU22" s="28"/>
+    </row>
+    <row r="23" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="A23" s="25"/>
+      <c r="B23" s="25"/>
+      <c r="U23" s="28"/>
+      <c r="V23" s="28"/>
+      <c r="W23" s="21"/>
+      <c r="X23" s="21"/>
+      <c r="AU23" s="28"/>
+    </row>
+    <row r="24" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="A24" s="25"/>
+      <c r="B24" s="25"/>
+      <c r="U24" s="28"/>
+      <c r="V24" s="28"/>
+      <c r="W24" s="21"/>
+      <c r="X24" s="21"/>
+      <c r="AU24" s="28"/>
+    </row>
+    <row r="25" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="A25" s="25"/>
+      <c r="B25" s="25"/>
+      <c r="U25" s="28"/>
+      <c r="V25" s="28"/>
+      <c r="W25" s="21"/>
+      <c r="X25" s="21"/>
+      <c r="AU25" s="28"/>
+    </row>
+    <row r="26" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="A26" s="25"/>
+      <c r="B26" s="25"/>
+      <c r="U26" s="28"/>
+      <c r="V26" s="28"/>
+      <c r="W26" s="21"/>
+      <c r="X26" s="21"/>
+      <c r="AU26" s="28"/>
+    </row>
+    <row r="27" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="A27" s="25"/>
+      <c r="B27" s="25"/>
+      <c r="U27" s="28"/>
+      <c r="V27" s="28"/>
+      <c r="W27" s="21"/>
+      <c r="X27" s="21"/>
+      <c r="AU27" s="28"/>
+    </row>
+    <row r="28" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="A28" s="21"/>
+      <c r="B28" s="21"/>
+      <c r="W28" s="21"/>
+      <c r="X28" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="AS2:AT2"/>
+    <mergeCell ref="AU2:AV2"/>
+    <mergeCell ref="AK2:AL2"/>
+    <mergeCell ref="AM2:AN2"/>
     <mergeCell ref="AO2:AP2"/>
     <mergeCell ref="AQ2:AR2"/>
-    <mergeCell ref="AS2:AT2"/>
-    <mergeCell ref="AU2:AV2"/>
+    <mergeCell ref="AA2:AB2"/>
+    <mergeCell ref="AC2:AD2"/>
     <mergeCell ref="AE2:AF2"/>
     <mergeCell ref="AG2:AH2"/>
     <mergeCell ref="AI2:AJ2"/>
-    <mergeCell ref="AK2:AL2"/>
-    <mergeCell ref="AM2:AN2"/>
+    <mergeCell ref="O2:T2"/>
     <mergeCell ref="U2:V2"/>
     <mergeCell ref="W2:X2"/>
     <mergeCell ref="Y2:Z2"/>
-    <mergeCell ref="AA2:AB2"/>
-    <mergeCell ref="AC2:AD2"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="E2:F2"/>
     <mergeCell ref="G2:H2"/>
     <mergeCell ref="I2:N2"/>
-    <mergeCell ref="O2:T2"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
   <legacyDrawing r:id="rId1"/>
@@ -1986,253 +3052,461 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Hoja3"/>
-  <dimension ref="A1:AB4"/>
+  <dimension ref="A1:AC28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="3" topLeftCell="T4" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="AB4" sqref="AB4"/>
+      <selection pane="bottomRight" activeCell="U5" sqref="U5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.7109375" customWidth="1"/>
     <col min="2" max="2" width="42.7109375" customWidth="1"/>
-    <col min="3" max="4" width="9.140625" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" customWidth="1"/>
+    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="26.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="10" width="9.140625" customWidth="1"/>
-    <col min="11" max="11" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="18" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="18" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="13.42578125" customWidth="1"/>
-    <col min="23" max="23" width="15.28515625" style="16" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="10.5703125" style="17" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="9.140625" customWidth="1"/>
+    <col min="10" max="10" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="25.28515625" customWidth="1"/>
+    <col min="21" max="21" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="28.85546875" customWidth="1"/>
+    <col min="23" max="23" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="C1" s="14" t="s">
+    <row r="1" spans="1:29" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="C1" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="D1" s="20" t="s">
         <v>65</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="E1" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="F1" s="15" t="s">
+      <c r="F1" s="20" t="s">
         <v>67</v>
       </c>
-      <c r="G1" s="14" t="s">
+      <c r="G1" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="H1" s="17"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="I1" s="11"/>
-      <c r="J1" s="10"/>
-      <c r="K1" s="14" t="s">
+      <c r="K1" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="L1" s="15" t="s">
+      <c r="L1" s="20" t="s">
         <v>71</v>
       </c>
-      <c r="M1" s="14" t="s">
+      <c r="M1" s="19" t="s">
         <v>72</v>
       </c>
-      <c r="N1" s="15" t="s">
+      <c r="N1" s="20" t="s">
         <v>73</v>
       </c>
-      <c r="O1" s="14" t="s">
+      <c r="O1" s="20" t="s">
         <v>74</v>
       </c>
-      <c r="P1" s="15" t="s">
+      <c r="P1" s="19" t="s">
         <v>75</v>
       </c>
-      <c r="Q1" s="14" t="s">
+      <c r="Q1" s="20" t="s">
         <v>76</v>
       </c>
-      <c r="R1" s="15" t="s">
+      <c r="R1" s="19" t="s">
         <v>77</v>
       </c>
-      <c r="S1" s="14" t="s">
+      <c r="S1" s="20" t="s">
         <v>78</v>
       </c>
-      <c r="T1" s="15" t="s">
+      <c r="T1" s="19" t="s">
+        <v>166</v>
+      </c>
+      <c r="U1" s="19" t="s">
         <v>79</v>
       </c>
-      <c r="U1" s="14" t="s">
+      <c r="V1" s="19" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="C2" s="64" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="C2" s="29" t="s">
+      <c r="D2" s="65" t="s">
         <v>81</v>
       </c>
-      <c r="D2" s="30" t="s">
+      <c r="E2" s="64" t="s">
         <v>82</v>
       </c>
-      <c r="E2" s="29" t="s">
+      <c r="F2" s="65" t="s">
         <v>83</v>
       </c>
-      <c r="F2" s="30" t="s">
+      <c r="G2" s="59" t="s">
         <v>84</v>
       </c>
-      <c r="G2" s="29" t="s">
+      <c r="H2" s="61"/>
+      <c r="I2" s="60"/>
+      <c r="J2" s="65" t="s">
         <v>85</v>
       </c>
-      <c r="H2" s="25" t="s">
+      <c r="K2" s="64" t="s">
         <v>86</v>
       </c>
-      <c r="I2" s="27"/>
-      <c r="J2" s="26"/>
-      <c r="K2" s="29" t="s">
+      <c r="L2" s="65" t="s">
         <v>87</v>
       </c>
-      <c r="L2" s="30" t="s">
+      <c r="M2" s="64" t="s">
         <v>88</v>
       </c>
-      <c r="M2" s="29" t="s">
+      <c r="N2" s="65" t="s">
         <v>89</v>
       </c>
-      <c r="N2" s="30" t="s">
+      <c r="O2" s="65" t="s">
         <v>90</v>
       </c>
-      <c r="O2" s="29" t="s">
+      <c r="P2" s="64" t="s">
         <v>91</v>
       </c>
-      <c r="P2" s="30" t="s">
+      <c r="Q2" s="65" t="s">
         <v>92</v>
       </c>
-      <c r="Q2" s="29" t="s">
+      <c r="R2" s="64" t="s">
         <v>93</v>
       </c>
-      <c r="R2" s="30" t="s">
+      <c r="S2" s="65" t="s">
         <v>94</v>
       </c>
-      <c r="S2" s="29" t="s">
+      <c r="T2" s="51" t="s">
+        <v>167</v>
+      </c>
+      <c r="U2" s="64" t="s">
         <v>95</v>
       </c>
-      <c r="T2" s="30" t="s">
+      <c r="V2" s="47" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A3" s="30" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="30" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="31" t="s">
+        <v>63</v>
+      </c>
+      <c r="D3" s="31" t="s">
+        <v>63</v>
+      </c>
+      <c r="E3" s="31" t="s">
+        <v>63</v>
+      </c>
+      <c r="F3" s="31" t="s">
+        <v>63</v>
+      </c>
+      <c r="G3" s="32" t="s">
         <v>96</v>
       </c>
-      <c r="U2" s="29" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="13" t="s">
+      <c r="H3" s="33" t="s">
+        <v>61</v>
+      </c>
+      <c r="I3" s="34" t="s">
         <v>63</v>
       </c>
-      <c r="D3" s="13" t="s">
+      <c r="J3" s="31" t="s">
         <v>63</v>
       </c>
-      <c r="E3" s="13" t="s">
+      <c r="K3" s="31" t="s">
         <v>63</v>
       </c>
-      <c r="F3" s="13" t="s">
+      <c r="L3" s="31" t="s">
         <v>63</v>
       </c>
-      <c r="G3" s="13" t="s">
+      <c r="M3" s="31" t="s">
         <v>63</v>
       </c>
-      <c r="H3" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="I3" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="J3" s="4" t="s">
+      <c r="N3" s="31" t="s">
         <v>63</v>
       </c>
-      <c r="K3" s="13" t="s">
+      <c r="O3" s="31" t="s">
         <v>63</v>
       </c>
-      <c r="L3" s="13" t="s">
+      <c r="P3" s="31" t="s">
         <v>63</v>
       </c>
-      <c r="M3" s="13" t="s">
+      <c r="Q3" s="31" t="s">
         <v>63</v>
       </c>
-      <c r="N3" s="13" t="s">
+      <c r="R3" s="31" t="s">
         <v>63</v>
       </c>
-      <c r="O3" s="13" t="s">
+      <c r="S3" s="31" t="s">
         <v>63</v>
       </c>
-      <c r="P3" s="13" t="s">
+      <c r="T3" s="48" t="s">
         <v>63</v>
       </c>
-      <c r="Q3" s="13" t="s">
+      <c r="U3" s="31" t="s">
         <v>63</v>
       </c>
-      <c r="R3" s="13" t="s">
+      <c r="V3" s="48" t="s">
         <v>63</v>
       </c>
-      <c r="S3" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="T3" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="U3" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="V3" s="20" t="s">
-        <v>106</v>
-      </c>
-      <c r="W3" s="20" t="s">
-        <v>107</v>
-      </c>
-      <c r="X3" s="20" t="s">
-        <v>108</v>
-      </c>
-      <c r="Y3" s="20" t="s">
-        <v>109</v>
-      </c>
-      <c r="Z3" s="20" t="s">
-        <v>110</v>
-      </c>
-      <c r="AA3" s="20" t="s">
-        <v>111</v>
-      </c>
-      <c r="AB3" s="20" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="AB4">
-        <f>+W4-X4-Z4-AA4</f>
+      <c r="W3" s="42" t="s">
+        <v>156</v>
+      </c>
+      <c r="X3" s="42" t="s">
+        <v>157</v>
+      </c>
+      <c r="Y3" s="42" t="s">
+        <v>158</v>
+      </c>
+      <c r="Z3" s="42" t="s">
+        <v>159</v>
+      </c>
+      <c r="AA3" s="42" t="s">
+        <v>160</v>
+      </c>
+      <c r="AB3" s="42" t="s">
+        <v>161</v>
+      </c>
+      <c r="AC3" s="42" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="4" spans="1:29" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="38"/>
+      <c r="B4" s="38"/>
+      <c r="C4" s="39"/>
+      <c r="N4" s="35"/>
+      <c r="P4" s="39"/>
+      <c r="T4" s="49"/>
+      <c r="Z4" s="37"/>
+      <c r="AC4" s="36">
+        <f>+X4-Y4-AA4-AB4</f>
         <v>0</v>
       </c>
     </row>
+    <row r="5" spans="1:29" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="38"/>
+      <c r="B5" s="38"/>
+      <c r="C5" s="39"/>
+      <c r="P5" s="39"/>
+      <c r="T5" s="49"/>
+      <c r="Z5" s="37"/>
+    </row>
+    <row r="6" spans="1:29" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="38"/>
+      <c r="B6" s="38"/>
+      <c r="C6" s="39"/>
+      <c r="P6" s="39"/>
+      <c r="T6" s="49"/>
+      <c r="Z6" s="37"/>
+    </row>
+    <row r="7" spans="1:29" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="38"/>
+      <c r="B7" s="38"/>
+      <c r="C7" s="39"/>
+      <c r="P7" s="39"/>
+      <c r="T7" s="49"/>
+      <c r="Z7" s="37"/>
+    </row>
+    <row r="8" spans="1:29" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="38"/>
+      <c r="B8" s="38"/>
+      <c r="C8" s="39"/>
+      <c r="P8" s="39"/>
+      <c r="T8" s="49"/>
+      <c r="Z8" s="37"/>
+    </row>
+    <row r="9" spans="1:29" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="38"/>
+      <c r="B9" s="38"/>
+      <c r="C9" s="39"/>
+      <c r="P9" s="39"/>
+      <c r="T9" s="49"/>
+      <c r="Z9" s="37"/>
+    </row>
+    <row r="10" spans="1:29" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="38"/>
+      <c r="B10" s="38"/>
+      <c r="C10" s="39"/>
+      <c r="P10" s="39"/>
+      <c r="T10" s="49"/>
+      <c r="Z10" s="37"/>
+    </row>
+    <row r="11" spans="1:29" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="38"/>
+      <c r="B11" s="38"/>
+      <c r="C11" s="39"/>
+      <c r="P11" s="39"/>
+      <c r="T11" s="49"/>
+      <c r="W11" s="40"/>
+      <c r="Z11" s="37"/>
+    </row>
+    <row r="12" spans="1:29" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="38"/>
+      <c r="B12" s="38"/>
+      <c r="C12" s="39"/>
+      <c r="P12" s="39"/>
+      <c r="T12" s="49"/>
+      <c r="Z12" s="37"/>
+    </row>
+    <row r="13" spans="1:29" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="38"/>
+      <c r="B13" s="38"/>
+      <c r="C13" s="39"/>
+      <c r="P13" s="39"/>
+      <c r="T13" s="49"/>
+      <c r="Z13" s="37"/>
+    </row>
+    <row r="14" spans="1:29" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="38"/>
+      <c r="B14" s="38"/>
+      <c r="C14" s="39"/>
+      <c r="P14" s="39"/>
+      <c r="T14" s="49"/>
+      <c r="Z14" s="37"/>
+    </row>
+    <row r="15" spans="1:29" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="38"/>
+      <c r="B15" s="38"/>
+      <c r="C15" s="39"/>
+      <c r="P15" s="39"/>
+      <c r="T15" s="49"/>
+      <c r="Z15" s="37"/>
+    </row>
+    <row r="16" spans="1:29" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="38"/>
+      <c r="B16" s="38"/>
+      <c r="C16" s="39"/>
+      <c r="P16" s="39"/>
+      <c r="T16" s="49"/>
+      <c r="Z16" s="37"/>
+    </row>
+    <row r="17" spans="1:26" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="38"/>
+      <c r="B17" s="38"/>
+      <c r="C17" s="39"/>
+      <c r="P17" s="39"/>
+      <c r="T17" s="49"/>
+      <c r="Z17" s="37"/>
+    </row>
+    <row r="18" spans="1:26" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="38"/>
+      <c r="B18" s="38"/>
+      <c r="C18" s="39"/>
+      <c r="P18" s="39"/>
+      <c r="T18" s="49"/>
+      <c r="Z18" s="37"/>
+    </row>
+    <row r="19" spans="1:26" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="38"/>
+      <c r="B19" s="38"/>
+      <c r="C19" s="39"/>
+      <c r="P19" s="39"/>
+      <c r="T19" s="49"/>
+      <c r="Z19" s="37"/>
+    </row>
+    <row r="20" spans="1:26" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="38"/>
+      <c r="B20" s="38"/>
+      <c r="C20" s="39"/>
+      <c r="P20" s="39"/>
+      <c r="T20" s="49"/>
+      <c r="Z20" s="37"/>
+    </row>
+    <row r="21" spans="1:26" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="38"/>
+      <c r="B21" s="38"/>
+      <c r="C21" s="39"/>
+      <c r="P21" s="39"/>
+      <c r="T21" s="49"/>
+      <c r="Z21" s="37"/>
+    </row>
+    <row r="22" spans="1:26" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="38"/>
+      <c r="B22" s="38"/>
+      <c r="C22" s="39"/>
+      <c r="P22" s="39"/>
+      <c r="T22" s="49"/>
+      <c r="Z22" s="37"/>
+    </row>
+    <row r="23" spans="1:26" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="38"/>
+      <c r="B23" s="38"/>
+      <c r="C23" s="39"/>
+      <c r="P23" s="39"/>
+      <c r="T23" s="50"/>
+      <c r="Z23" s="37"/>
+    </row>
+    <row r="24" spans="1:26" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="38"/>
+      <c r="B24" s="38"/>
+      <c r="C24" s="39"/>
+      <c r="P24" s="39"/>
+      <c r="T24" s="49"/>
+      <c r="Z24" s="37"/>
+    </row>
+    <row r="25" spans="1:26" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="38"/>
+      <c r="B25" s="38"/>
+      <c r="C25" s="39"/>
+      <c r="P25" s="39"/>
+      <c r="T25" s="49"/>
+      <c r="Z25" s="37"/>
+    </row>
+    <row r="26" spans="1:26" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="38"/>
+      <c r="B26" s="38"/>
+      <c r="C26" s="39"/>
+      <c r="P26" s="39"/>
+      <c r="T26" s="49"/>
+      <c r="Z26" s="37"/>
+    </row>
+    <row r="27" spans="1:26" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="38"/>
+      <c r="B27" s="38"/>
+      <c r="C27" s="39"/>
+      <c r="P27" s="39"/>
+      <c r="T27"/>
+      <c r="Z27" s="37"/>
+    </row>
+    <row r="28" spans="1:26" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="41"/>
+      <c r="B28" s="41"/>
+      <c r="T28"/>
+      <c r="Z28" s="37"/>
+    </row>
   </sheetData>
-  <mergeCells count="17">
-    <mergeCell ref="T2"/>
+  <mergeCells count="16">
+    <mergeCell ref="S2"/>
     <mergeCell ref="U2"/>
     <mergeCell ref="O2"/>
     <mergeCell ref="P2"/>
     <mergeCell ref="Q2"/>
     <mergeCell ref="R2"/>
-    <mergeCell ref="S2"/>
-    <mergeCell ref="H2:J2"/>
+    <mergeCell ref="J2"/>
     <mergeCell ref="K2"/>
     <mergeCell ref="L2"/>
     <mergeCell ref="M2"/>
@@ -2241,7 +3515,7 @@
     <mergeCell ref="D2"/>
     <mergeCell ref="E2"/>
     <mergeCell ref="F2"/>
-    <mergeCell ref="G2"/>
+    <mergeCell ref="G2:I2"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
   <legacyDrawing r:id="rId1"/>
@@ -2250,57 +3524,147 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Hoja4"/>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:D29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="E11" sqref="E11"/>
+      <selection pane="bottomRight" activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.7109375" customWidth="1"/>
     <col min="2" max="2" width="42.7109375" customWidth="1"/>
-    <col min="4" max="4" width="24.28515625" customWidth="1"/>
-    <col min="5" max="5" width="23.85546875" customWidth="1"/>
+    <col min="4" max="4" width="16.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="C1" s="7" t="s">
+    <row r="1" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="C1" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="D1" s="14"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C2" s="59" t="s">
+        <v>98</v>
+      </c>
+      <c r="D2" s="60"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="30" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="30"/>
+      <c r="C3" s="32" t="s">
+        <v>63</v>
+      </c>
+      <c r="D3" s="34" t="s">
         <v>99</v>
       </c>
-      <c r="D1" s="8"/>
-      <c r="E1" s="15" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C2" s="23" t="s">
-        <v>100</v>
-      </c>
-      <c r="D2" s="24"/>
-      <c r="E2" s="19" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="E3" s="13" t="s">
-        <v>63</v>
-      </c>
-    </row>
+    </row>
+    <row r="4" spans="1:4" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="38"/>
+      <c r="B4" s="38"/>
+    </row>
+    <row r="5" spans="1:4" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="38"/>
+      <c r="B5" s="38"/>
+    </row>
+    <row r="6" spans="1:4" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="38"/>
+      <c r="B6" s="38"/>
+    </row>
+    <row r="7" spans="1:4" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="38"/>
+      <c r="B7" s="38"/>
+    </row>
+    <row r="8" spans="1:4" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="38"/>
+      <c r="B8" s="38"/>
+    </row>
+    <row r="9" spans="1:4" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="38"/>
+      <c r="B9" s="38"/>
+    </row>
+    <row r="10" spans="1:4" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="38"/>
+      <c r="B10" s="38"/>
+    </row>
+    <row r="11" spans="1:4" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="38"/>
+      <c r="B11" s="38"/>
+    </row>
+    <row r="12" spans="1:4" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="38"/>
+      <c r="B12" s="38"/>
+    </row>
+    <row r="13" spans="1:4" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="38"/>
+      <c r="B13" s="38"/>
+    </row>
+    <row r="14" spans="1:4" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="38"/>
+      <c r="B14" s="38"/>
+    </row>
+    <row r="15" spans="1:4" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="38"/>
+      <c r="B15" s="38"/>
+    </row>
+    <row r="16" spans="1:4" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="38"/>
+      <c r="B16" s="38"/>
+    </row>
+    <row r="17" spans="1:2" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="38"/>
+      <c r="B17" s="38"/>
+    </row>
+    <row r="18" spans="1:2" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="38"/>
+      <c r="B18" s="38"/>
+    </row>
+    <row r="19" spans="1:2" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="38"/>
+      <c r="B19" s="38"/>
+    </row>
+    <row r="20" spans="1:2" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="38"/>
+      <c r="B20" s="38"/>
+    </row>
+    <row r="21" spans="1:2" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="38"/>
+      <c r="B21" s="38"/>
+    </row>
+    <row r="22" spans="1:2" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="38"/>
+      <c r="B22" s="38"/>
+    </row>
+    <row r="23" spans="1:2" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="38"/>
+      <c r="B23" s="38"/>
+    </row>
+    <row r="24" spans="1:2" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="38"/>
+      <c r="B24" s="38"/>
+    </row>
+    <row r="25" spans="1:2" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="38"/>
+      <c r="B25" s="38"/>
+    </row>
+    <row r="26" spans="1:2" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="38"/>
+      <c r="B26" s="38"/>
+    </row>
+    <row r="27" spans="1:2" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="38"/>
+      <c r="B27" s="38"/>
+    </row>
+    <row r="28" spans="1:2" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="41"/>
+      <c r="B28" s="41"/>
+    </row>
+    <row r="29" spans="1:2" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="C2:D2"/>

</xml_diff>